<commit_message>
Added Backoffice retail, onlineoutlet stores
</commit_message>
<xml_diff>
--- a/NewArrivals/timezoneData.xlsx
+++ b/NewArrivals/timezoneData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\CabiClio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\TestAutomation\NewArrivals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Integrated addon personal order and warehouse shipping
</commit_message>
<xml_diff>
--- a/NewArrivals/timezoneData.xlsx
+++ b/NewArrivals/timezoneData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\TestAutomation\NewArrivals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\NewArrivals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
   <si>
     <t>orderType</t>
   </si>
@@ -62,9 +62,6 @@
     <t>BOPersonal</t>
   </si>
   <si>
-    <t>BOAddon</t>
-  </si>
-  <si>
     <t>BORetail</t>
   </si>
   <si>
@@ -93,6 +90,12 @@
   </si>
   <si>
     <t>test14</t>
+  </si>
+  <si>
+    <t>BOAddonPersonal</t>
+  </si>
+  <si>
+    <t>BOAddonRetail</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,9 +432,11 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -445,33 +450,36 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -480,36 +488,39 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -518,36 +529,39 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -556,36 +570,39 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -594,31 +611,34 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>